<commit_message>
map and planning files added
</commit_message>
<xml_diff>
--- a/_planning/perkinites.xlsx
+++ b/_planning/perkinites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
   <si>
     <t>NC</t>
   </si>
@@ -493,6 +493,27 @@
   </si>
   <si>
     <t>DR</t>
+  </si>
+  <si>
+    <t>Healing Staff</t>
+  </si>
+  <si>
+    <t>Heal</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Healthy Explosion</t>
+  </si>
+  <si>
+    <t>120 points shield</t>
+  </si>
+  <si>
+    <t>Heals target (could be self)</t>
+  </si>
+  <si>
+    <t>Damages close target</t>
   </si>
 </sst>
 </file>
@@ -837,9 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1109,7 +1130,9 @@
       <c r="D11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>100</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1312,7 +1335,9 @@
         <v>122</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>20</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1667,8 +1692,12 @@
         <v>19</v>
       </c>
       <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" s="1">
+        <v>20</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -1684,6 +1713,51 @@
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
+    </row>
+    <row r="60" spans="1:24">
+      <c r="A60" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60">
+        <v>70</v>
+      </c>
+      <c r="E60">
+        <v>300</v>
+      </c>
+      <c r="J60" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="N60" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24">
+      <c r="A61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D61">
+        <v>50</v>
+      </c>
+      <c r="N61" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24">
+      <c r="A62" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62">
+        <v>80</v>
+      </c>
+      <c r="E62">
+        <v>30</v>
+      </c>
+      <c r="F62">
+        <v>70</v>
+      </c>
+      <c r="N62" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="63" spans="1:24">
       <c r="A63" s="1" t="s">

</xml_diff>

<commit_message>
multiple editor and planning changes
</commit_message>
<xml_diff>
--- a/_planning/perkinites.xlsx
+++ b/_planning/perkinites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
   <si>
     <t>NC</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Vivian Hsiao</t>
   </si>
   <si>
-    <t>Pencil</t>
-  </si>
-  <si>
     <t>Hulk Rage</t>
   </si>
   <si>
@@ -514,6 +511,42 @@
   </si>
   <si>
     <t>Damages close target</t>
+  </si>
+  <si>
+    <t>Claws</t>
+  </si>
+  <si>
+    <t>Shockwave</t>
+  </si>
+  <si>
+    <t>Machine gun</t>
+  </si>
+  <si>
+    <t>Overload</t>
+  </si>
+  <si>
+    <t>Bio-leech</t>
+  </si>
+  <si>
+    <t>Damages enemies in a wave</t>
+  </si>
+  <si>
+    <t>Drain HP from target enemy</t>
+  </si>
+  <si>
+    <t>After channeling, unleash massive damage to nearby enemies</t>
+  </si>
+  <si>
+    <t>Orgo Textbook</t>
+  </si>
+  <si>
+    <t>Maul</t>
+  </si>
+  <si>
+    <t>Silent Treatment</t>
+  </si>
+  <si>
+    <t>"That's What She Said"</t>
   </si>
 </sst>
 </file>
@@ -858,9 +891,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N63" sqref="N63"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A75:D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -881,19 +914,19 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1"/>
       <c r="H1" s="1"/>
@@ -903,63 +936,63 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="1">
         <v>50</v>
@@ -977,7 +1010,7 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
@@ -985,7 +1018,7 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -997,12 +1030,12 @@
         <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -1023,15 +1056,15 @@
         <v>0.3</v>
       </c>
       <c r="N5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -1045,10 +1078,10 @@
         <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="T6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="1" customFormat="1">
@@ -1059,15 +1092,15 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:24">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8">
         <v>50</v>
@@ -1082,12 +1115,12 @@
         <v>18</v>
       </c>
       <c r="N8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9">
         <v>24</v>
@@ -1099,12 +1132,12 @@
         <v>40</v>
       </c>
       <c r="N9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10">
         <v>70</v>
@@ -1114,21 +1147,21 @@
       </c>
       <c r="F10" s="2"/>
       <c r="N10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" s="1">
         <v>100</v>
@@ -1144,14 +1177,14 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
       <c r="T11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -1163,12 +1196,12 @@
         <v>15</v>
       </c>
       <c r="N12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D13">
         <v>24</v>
@@ -1183,12 +1216,12 @@
         <v>0.15</v>
       </c>
       <c r="N13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14">
         <v>110</v>
@@ -1197,18 +1230,18 @@
         <v>20</v>
       </c>
       <c r="N14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1226,7 +1259,7 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16">
         <v>100</v>
@@ -1238,40 +1271,40 @@
         <v>35</v>
       </c>
       <c r="N16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17">
         <v>60</v>
       </c>
       <c r="N17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" t="s">
+        <v>116</v>
+      </c>
+      <c r="N18" t="s">
         <v>117</v>
-      </c>
-      <c r="N18" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1293,7 +1326,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1301,26 +1334,26 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I26" s="3">
         <v>-0.2</v>
       </c>
       <c r="N26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P26" s="1"/>
     </row>
@@ -1332,9 +1365,11 @@
         <v>15</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="E27" s="1">
         <v>20</v>
       </c>
@@ -1351,17 +1386,17 @@
       <c r="P27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E28">
         <v>30</v>
@@ -1370,12 +1405,12 @@
         <v>10</v>
       </c>
       <c r="N28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29">
         <v>120</v>
@@ -1390,21 +1425,21 @@
         <v>20</v>
       </c>
       <c r="N29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:22">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D30">
         <v>50</v>
       </c>
       <c r="L30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:22">
@@ -1415,10 +1450,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E31" s="1">
         <v>50</v>
@@ -1436,14 +1471,14 @@
       <c r="P31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
     </row>
     <row r="32" spans="1:22">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32">
         <v>80</v>
@@ -1455,15 +1490,15 @@
         <v>20</v>
       </c>
       <c r="N32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33">
         <v>140</v>
@@ -1475,15 +1510,15 @@
         <v>0.5</v>
       </c>
       <c r="N33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D34">
         <v>30</v>
@@ -1492,24 +1527,24 @@
         <v>150</v>
       </c>
       <c r="N34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="T34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E35" s="1">
         <v>30</v>
@@ -1525,13 +1560,13 @@
       <c r="Q35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U35" s="1"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36">
         <v>50</v>
@@ -1543,26 +1578,26 @@
         <v>50</v>
       </c>
       <c r="N36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D37">
         <v>230</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C38">
         <v>150</v>
@@ -1577,15 +1612,15 @@
         <v>0.3</v>
       </c>
       <c r="N38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -1605,53 +1640,53 @@
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:21">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:24">
@@ -1662,7 +1697,7 @@
         <v>17</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1672,10 +1707,10 @@
     </row>
     <row r="55" spans="1:24">
       <c r="A55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -1693,7 +1728,7 @@
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E59" s="1">
         <v>20</v>
@@ -1716,7 +1751,7 @@
     </row>
     <row r="60" spans="1:24">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D60">
         <v>70</v>
@@ -1728,23 +1763,23 @@
         <v>0.25</v>
       </c>
       <c r="N60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:24">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D61">
         <v>50</v>
       </c>
       <c r="N61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:24">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D62">
         <v>80</v>
@@ -1756,12 +1791,12 @@
         <v>70</v>
       </c>
       <c r="N62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:24">
       <c r="A63" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1845,7 +1880,7 @@
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>28</v>
+        <v>173</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -1864,6 +1899,21 @@
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
     </row>
+    <row r="76" spans="1:22">
+      <c r="A76" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22">
+      <c r="A77" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22">
+      <c r="A78" t="s">
+        <v>176</v>
+      </c>
+    </row>
     <row r="79" spans="1:22">
       <c r="A79" s="1" t="s">
         <v>8</v>
@@ -1872,7 +1922,7 @@
         <v>7</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -1894,13 +1944,13 @@
     </row>
     <row r="83" spans="1:23">
       <c r="A83" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C83" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -1921,26 +1971,26 @@
     </row>
     <row r="84" spans="1:23">
       <c r="A84" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N84" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="1:23">
       <c r="A85" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:23">
       <c r="A87" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B87" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -1985,18 +2035,18 @@
     </row>
     <row r="92" spans="1:23">
       <c r="A92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N92" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:23">
       <c r="A93" t="s">
+        <v>36</v>
+      </c>
+      <c r="N93" t="s">
         <v>37</v>
-      </c>
-      <c r="N93" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:23">
@@ -2025,7 +2075,7 @@
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:14">
       <c r="A99" s="1" t="s">
         <v>10</v>
       </c>
@@ -2038,22 +2088,47 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="100" spans="1:14">
+      <c r="A100" t="s">
+        <v>166</v>
+      </c>
+      <c r="N100" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101" t="s">
+        <v>169</v>
+      </c>
+      <c r="N101" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" t="s">
+        <v>168</v>
+      </c>
+      <c r="N102" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
       <c r="A103" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="D103" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="107" spans="1:7" s="1" customFormat="1"/>
-    <row r="111" spans="1:7" s="1" customFormat="1"/>
-    <row r="112" spans="1:7">
+    <row r="107" spans="1:14" s="1" customFormat="1"/>
+    <row r="111" spans="1:14" s="1" customFormat="1"/>
+    <row r="112" spans="1:14">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>

</xml_diff>

<commit_message>
Trying to prepare for more Map implementation.
</commit_message>
<xml_diff>
--- a/_planning/perkinites.xlsx
+++ b/_planning/perkinites.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="202">
   <si>
     <t>NC</t>
   </si>
@@ -547,6 +547,81 @@
   </si>
   <si>
     <t>"That's What She Said"</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>Mauricio Pinilla</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>Ariana Gunderson</t>
+  </si>
+  <si>
+    <t>Claudine Yee</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>CY2</t>
+  </si>
+  <si>
+    <t>Teddy Bear Hug</t>
+  </si>
+  <si>
+    <t>Febreeze Spraying</t>
+  </si>
+  <si>
+    <t>Mummy Curse</t>
+  </si>
+  <si>
+    <t>Orgo 2 Textbook</t>
+  </si>
+  <si>
+    <t>Hair Flip</t>
+  </si>
+  <si>
+    <t>Cupcake Launcher</t>
+  </si>
+  <si>
+    <t>Access Denied</t>
+  </si>
+  <si>
+    <t>Swap Attire</t>
+  </si>
+  <si>
+    <t>Foreign Languages</t>
+  </si>
+  <si>
+    <t>Opera Piercing</t>
+  </si>
+  <si>
+    <t>Whip hair to the side to create a damaging sonic boom.</t>
+  </si>
+  <si>
+    <t>Modify your Attack and Speed with new clothes. Also increase Health…somehow.</t>
+  </si>
+  <si>
+    <t>Gets up close and squeezes target enemy with kindness. :)</t>
+  </si>
+  <si>
+    <t>Sprays Febreeze in a cone, creating the sense of freshness!</t>
+  </si>
+  <si>
+    <t>Wrap an opponent in bandages. Also status downgrades.</t>
+  </si>
+  <si>
+    <t>Confuse enemies around you.</t>
+  </si>
+  <si>
+    <t>Create a barrage of hot cupcakes.</t>
+  </si>
+  <si>
+    <t>Deny access to the Sci Li. Stuns enemies. If in the Sci Li, increases Ariana's and Claudine's Attack.</t>
   </si>
 </sst>
 </file>
@@ -892,8 +967,8 @@
   <dimension ref="A1:X135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A75:D79"/>
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2126,25 +2201,117 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="107" spans="1:14" s="1" customFormat="1"/>
-    <row r="111" spans="1:14" s="1" customFormat="1"/>
+    <row r="106" spans="1:14">
+      <c r="A106" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" s="1" customFormat="1">
+      <c r="A107" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="A108" t="s">
+        <v>184</v>
+      </c>
+      <c r="N108" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" t="s">
+        <v>185</v>
+      </c>
+      <c r="N109" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="A110" t="s">
+        <v>188</v>
+      </c>
+      <c r="N110" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" s="1" customFormat="1">
+      <c r="A111" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
     <row r="112" spans="1:14">
-      <c r="A112" s="1"/>
+      <c r="A112" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
-    </row>
-    <row r="115" spans="21:22">
+      <c r="N112" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="113" spans="1:22">
+      <c r="A113" t="s">
+        <v>191</v>
+      </c>
+      <c r="N113" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="114" spans="1:22">
+      <c r="A114" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="N114" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22">
+      <c r="A115" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="U115" s="1"/>
       <c r="V115" s="1"/>
     </row>
-    <row r="119" spans="21:22">
+    <row r="116" spans="1:22">
+      <c r="A116" t="s">
+        <v>189</v>
+      </c>
+      <c r="N116" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22">
+      <c r="A117" t="s">
+        <v>190</v>
+      </c>
+      <c r="N117" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="119" spans="1:22">
       <c r="U119" s="1"/>
       <c r="V119" s="1"/>
     </row>
-    <row r="123" spans="21:22">
+    <row r="123" spans="1:22">
       <c r="U123" s="1"/>
     </row>
-    <row r="127" spans="21:22">
+    <row r="127" spans="1:22">
       <c r="U127" s="1"/>
       <c r="V127" s="1"/>
     </row>

</xml_diff>